<commit_message>
Generate and save output file after processing
</commit_message>
<xml_diff>
--- a/output_cds/brown university.xlsx
+++ b/output_cds/brown university.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,70 +521,85 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
+          <t>general_college_subjects.history</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>general_college_subjects.electives</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>general_college_subjects.cs</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
           <t>general_college_subjects.arts</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>sat_act_required.sat_or_act</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>sat_act_required.sat only</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>sat_act_required.act only</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>residency_acceptance.in-state</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>residency_acceptance.out-of-state</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>residency_acceptance.international</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>residency_acceptance.others</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>sat_scores.25th</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>sat_scores.50th</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>sat_scores.75th</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>act scores.25th</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>act scores.50th</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>act scores.75th</t>
         </is>
@@ -604,37 +619,37 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -661,39 +676,48 @@
         <v>0</v>
       </c>
       <c r="R2" t="n">
+        <v>2</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
         <v>0</v>
       </c>
-      <c r="S2" t="b">
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="b">
         <v>1</v>
       </c>
-      <c r="T2" t="b">
+      <c r="W2" t="b">
         <v>0</v>
       </c>
-      <c r="U2" t="b">
+      <c r="X2" t="b">
         <v>0</v>
       </c>
-      <c r="V2" t="n">
+      <c r="Y2" t="n">
         <v>0.05394241779813512</v>
       </c>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="n">
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="n">
         <v>1510</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AD2" t="n">
         <v>1540</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AE2" t="n">
         <v>1560</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AF2" t="n">
         <v>34</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AG2" t="n">
         <v>35</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AH2" t="n">
         <v>35</v>
       </c>
     </row>

</xml_diff>